<commit_message>
updated theme and read depth limit to graph
</commit_message>
<xml_diff>
--- a/run_kits.xlsx
+++ b/run_kits.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ft22092_bristol_ac_uk/Documents/Git_repo/ShinySeq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="8_{54A77C2E-E3E5-5C42-B22C-B6ADCDEDD3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8036B9C3-D381-2A41-98BF-61921AEA07DE}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{54A77C2E-E3E5-5C42-B22C-B6ADCDEDD3F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B1735B-33C1-E04D-BF63-EA7AEC2FFBFD}"/>
   <bookViews>
     <workbookView xWindow="9460" yWindow="820" windowWidth="19680" windowHeight="17440" xr2:uid="{72DB86E6-C9ED-A64E-BC9C-1251E84745EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>KitName</t>
   </si>
@@ -69,6 +69,30 @@
   </si>
   <si>
     <t>NextSeq 2000 P2 (100 Cycles) </t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>400 M</t>
+  </si>
+  <si>
+    <t>130 M</t>
+  </si>
+  <si>
+    <t>1.8 B</t>
+  </si>
+  <si>
+    <t>200 M</t>
+  </si>
+  <si>
+    <t>800 M</t>
+  </si>
+  <si>
+    <t>2.4 B</t>
+  </si>
+  <si>
+    <t>3.6 B</t>
   </si>
 </sst>
 </file>
@@ -473,18 +497,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEBC3D1-7354-1344-BE61-4220FCD565F7}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +519,11 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -505,30 +533,41 @@
       <c r="C2" s="4">
         <v>1607.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="6">
-        <v>260000000</v>
+        <f>260000000/2</f>
+        <v>130000000</v>
       </c>
       <c r="C3" s="4">
         <v>1173.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>800000000</v>
+        <f>800000001/2</f>
+        <v>400000000.5</v>
       </c>
       <c r="C4" s="4">
         <v>3079.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -538,8 +577,11 @@
       <c r="C5" s="7">
         <v>2150</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -549,8 +591,11 @@
       <c r="C6" s="7">
         <v>645</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -560,8 +605,11 @@
       <c r="C7" s="7">
         <v>986</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -571,8 +619,11 @@
       <c r="C8" s="7">
         <v>2122</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -581,6 +632,9 @@
       </c>
       <c r="C9" s="7">
         <v>2986</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
default data and toggles
</commit_message>
<xml_diff>
--- a/run_kits.xlsx
+++ b/run_kits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10125"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ft22092_bristol_ac_uk/Documents/Git_repo/ShinySeq/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="14_{17B73A5F-5D38-FB4F-A039-BCAFCD8832F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D49E3F2E-9AE3-3F4E-98C0-FAE8F34D3633}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="14_{17B73A5F-5D38-FB4F-A039-BCAFCD8832F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{383ADFA0-D4B7-174C-AE0E-58411DBC23A8}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="1440" windowWidth="19680" windowHeight="17440" xr2:uid="{72DB86E6-C9ED-A64E-BC9C-1251E84745EA}"/>
+    <workbookView xWindow="17520" yWindow="2760" windowWidth="19680" windowHeight="17440" xr2:uid="{72DB86E6-C9ED-A64E-BC9C-1251E84745EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>KitName</t>
   </si>
@@ -59,39 +59,12 @@
     <t>NextSeq 2000 P4 (50 Cycles)</t>
   </si>
   <si>
-    <t>NextSeq 2000 P3 (100 Cycles) </t>
-  </si>
-  <si>
-    <t>NextSeq 2000 P4 (100 Cycles) </t>
-  </si>
-  <si>
-    <t>NextSeq 2000 P1 (100 Cycles) </t>
-  </si>
-  <si>
-    <t>NextSeq 2000 P2 (100 Cycles) </t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
     <t>400 M</t>
   </si>
   <si>
-    <t>200 M</t>
-  </si>
-  <si>
-    <t>800 M</t>
-  </si>
-  <si>
-    <t>2.4 B</t>
-  </si>
-  <si>
-    <t>3.6 B</t>
-  </si>
-  <si>
-    <t>260 M</t>
-  </si>
-  <si>
     <t>90 M</t>
   </si>
   <si>
@@ -126,6 +99,30 @@
   </si>
   <si>
     <t>NovaSeq X</t>
+  </si>
+  <si>
+    <t>130 M</t>
+  </si>
+  <si>
+    <t>100 M</t>
+  </si>
+  <si>
+    <t>1.2 B</t>
+  </si>
+  <si>
+    <t>1.8 B</t>
+  </si>
+  <si>
+    <t>NextSeq 2000 P4 (100 Cycles)</t>
+  </si>
+  <si>
+    <t>NextSeq 2000 P3 (100 Cycles)</t>
+  </si>
+  <si>
+    <t>NextSeq 2000 P2 (100 Cycles)</t>
+  </si>
+  <si>
+    <t>NextSeq 2000 P1 (100 Cycles)</t>
   </si>
 </sst>
 </file>
@@ -187,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -196,7 +193,6 @@
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +530,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="C7:D9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,7 +542,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -558,15 +554,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -578,7 +574,7 @@
         <v>1607.4</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F2" s="7">
         <f>D2/C2</f>
@@ -587,7 +583,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>5</v>
@@ -599,7 +595,7 @@
         <v>1173.25</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F3" s="7">
         <f t="shared" ref="F3:F12" si="0">D3/C3</f>
@@ -608,7 +604,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>3</v>
@@ -620,7 +616,7 @@
         <v>3079.9</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="F4" s="7">
         <f t="shared" si="0"/>
@@ -629,123 +625,116 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="5">
-        <v>900000000</v>
+      <c r="C5" s="7">
+        <v>100000000</v>
       </c>
       <c r="D5" s="6">
-        <v>2150</v>
+        <v>645</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>2.3888888888888887E-6</v>
+        <v>6.4500000000000001E-6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7">
-        <v>100000000</v>
+        <v>400000002</v>
       </c>
       <c r="D6" s="6">
-        <v>645</v>
+        <v>986</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="F6" s="7">
         <f t="shared" si="0"/>
-        <v>6.4500000000000001E-6</v>
-      </c>
+        <v>2.4649999876749999E-6</v>
+      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C7" s="7">
-        <v>400000002</v>
+        <v>1200000000</v>
       </c>
       <c r="D7" s="6">
-        <v>986</v>
+        <v>2122</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="F7" s="7">
         <f t="shared" si="0"/>
-        <v>2.4649999876749999E-6</v>
-      </c>
-      <c r="G7" s="8">
-        <f>D7/D9</f>
-        <v>0.3302076356329538</v>
-      </c>
-      <c r="H7" s="7">
-        <f>C7/C9</f>
-        <v>0.22222222333333333</v>
+        <v>1.7683333333333333E-6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C8" s="7">
-        <v>1200000000</v>
+        <v>1800000000</v>
       </c>
       <c r="D8" s="6">
-        <v>2122</v>
+        <v>2986</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F8" s="7">
         <f t="shared" si="0"/>
-        <v>1.7683333333333333E-6</v>
+        <v>1.6588888888888889E-6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" s="7">
         <v>1800000000</v>
       </c>
       <c r="D9" s="6">
-        <v>2986</v>
+        <v>2150</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="0"/>
-        <v>1.6588888888888889E-6</v>
+        <f>D9/C9</f>
+        <v>1.1944444444444443E-6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C10" s="7">
         <v>1600000000</v>
@@ -754,7 +743,7 @@
         <v>1713</v>
       </c>
       <c r="E10" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="F10" s="7">
         <f t="shared" si="0"/>
@@ -763,10 +752,10 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C11" s="7">
         <v>10000000000</v>
@@ -775,7 +764,7 @@
         <v>6399</v>
       </c>
       <c r="E11" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="F11" s="7">
         <f t="shared" si="0"/>
@@ -784,10 +773,10 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C12" s="7">
         <v>26000000000</v>
@@ -796,7 +785,7 @@
         <v>10233</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="F12" s="7">
         <f t="shared" si="0"/>
@@ -804,16 +793,6 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F2:F12">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C2:C12">
     <cfRule type="colorScale" priority="2">
       <colorScale>
@@ -834,6 +813,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F12">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>